<commit_message>
Add more test data Update README.md Refactor tests
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/navigation.xlsx
+++ b/src/test/resources/test-data/navigation.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sewwandi_j/Documents/Documents/Projects/Automation/ui-automation/src/test/resources/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0AC546-3DFD-E84F-857B-B71BB5E6B1EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3553CF-0AE5-2F44-9AAA-6DA61A4054A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="30760" windowHeight="17440" xr2:uid="{653006DF-B906-2D46-AD81-C3D37115229D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Products" sheetId="1" r:id="rId1"/>
-    <sheet name="Categories2" sheetId="2" r:id="rId2"/>
-    <sheet name="Electronic Devices (2)" sheetId="5" r:id="rId3"/>
+    <sheet name="Products" sheetId="6" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
   <si>
     <t>Electronic Devices</t>
   </si>
@@ -84,6 +82,114 @@
   </si>
   <si>
     <t>394798495</t>
+  </si>
+  <si>
+    <t>668320174</t>
+  </si>
+  <si>
+    <t>Power Banks</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Headphones &amp; Headsets</t>
+  </si>
+  <si>
+    <t>Headphones and Headsets</t>
+  </si>
+  <si>
+    <t>Desktops Computers</t>
+  </si>
+  <si>
+    <t>All-In-One</t>
+  </si>
+  <si>
+    <t>All-in-One Desktop</t>
+  </si>
+  <si>
+    <t>Tablets</t>
+  </si>
+  <si>
+    <t>Gaming Consoles</t>
+  </si>
+  <si>
+    <t>PlayStation Consoles</t>
+  </si>
+  <si>
+    <t>Console Gaming Consoles</t>
+  </si>
+  <si>
+    <t>Action/Video Cameras</t>
+  </si>
+  <si>
+    <t>Professional Video Camera</t>
+  </si>
+  <si>
+    <t>Gadgets &amp; Drones</t>
+  </si>
+  <si>
+    <t>Drones</t>
+  </si>
+  <si>
+    <t>Media Players</t>
+  </si>
+  <si>
+    <t>Walkie-Talkies</t>
+  </si>
+  <si>
+    <t>Gadgets Walkie Talkies</t>
+  </si>
+  <si>
+    <t>2-in-1s</t>
+  </si>
+  <si>
+    <t>2 In 1 Laptops</t>
+  </si>
+  <si>
+    <t>Gaming Desktops</t>
+  </si>
+  <si>
+    <t>DIY</t>
+  </si>
+  <si>
+    <t>DIY Desktop</t>
+  </si>
+  <si>
+    <t>Playstation Games</t>
+  </si>
+  <si>
+    <t>Console Games</t>
+  </si>
+  <si>
+    <t>Playstation Controllers</t>
+  </si>
+  <si>
+    <t>Console Gaming Controllers</t>
+  </si>
+  <si>
+    <t>Nintendo Consoles</t>
+  </si>
+  <si>
+    <t>Nintendo Games</t>
+  </si>
+  <si>
+    <t>Nintendo Joy-Cons</t>
+  </si>
+  <si>
+    <t>Nintendo Screen Protectors</t>
+  </si>
+  <si>
+    <t>Console Gaming Accessories Screen Protectors</t>
+  </si>
+  <si>
+    <t>Xbox Consoles</t>
+  </si>
+  <si>
+    <t>Xbox Games</t>
+  </si>
+  <si>
+    <t>Other Gaming Consoles</t>
   </si>
 </sst>
 </file>
@@ -144,15 +250,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,19 +570,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B4660E-6ABC-CC42-ABFF-040211773BFA}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9569E2-5311-CC4E-A27A-D3AC344A2A33}">
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
@@ -497,11 +601,11 @@
       <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -513,10 +617,10 @@
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>342420759</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -533,7 +637,7 @@
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>568942261</v>
       </c>
     </row>
@@ -550,11 +654,11 @@
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>1244390456</v>
       </c>
-      <c r="F4" s="6">
-        <v>1221476592</v>
+      <c r="F4" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G4" s="3">
         <v>1007886215</v>
@@ -573,278 +677,333 @@
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>661442361</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>509918490</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1">
+        <v>507998277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1">
+        <v>319336369</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1">
+        <v>584934349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1159552504</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1241890567</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="1">
+        <v>871112807</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1">
+        <v>862742128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="1">
+        <v>282557279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="1">
+        <v>561488196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B395FD26-BB05-AC43-BDB0-3669365B7874}">
-  <dimension ref="A1:H15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.5" style="1" customWidth="1"/>
-    <col min="2" max="3" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1D7606-5EDB-4845-A149-48B21A447139}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
-        <v>1243892091</v>
-      </c>
-      <c r="B2" s="4">
-        <v>568942261</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1244390456</v>
-      </c>
-      <c r="D2" s="4">
-        <v>661442361</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>394798495</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1221476592</v>
-      </c>
-      <c r="D3" s="1">
-        <v>509918490</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="1">
-        <v>996692606</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1243892091</v>
-      </c>
-      <c r="C7" s="5">
-        <v>394798495</v>
-      </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="5">
-        <v>568942261</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="6">
-        <v>1244390456</v>
-      </c>
-      <c r="C9" s="6">
-        <v>1221476592</v>
-      </c>
-      <c r="D9" s="6">
-        <v>996692606</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5">
-        <v>661442361</v>
-      </c>
-      <c r="C10" s="6">
-        <v>509918490</v>
-      </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>